<commit_message>
Update plots and tables
</commit_message>
<xml_diff>
--- a/Summary CATE Metrics.xlsx
+++ b/Summary CATE Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shelbygolden/Desktop/Life/Personal/College/Masters/Johns Hopkins/Statistical Theory II/Stat Theory II_Spring 2023/Semester Project/Project GitHub Repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F7EA50-76AD-F64B-962E-5A174EDE22BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41960F8-BBEA-3347-98CB-9FB30AA2513E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16640" activeTab="1" xr2:uid="{60BB6ECC-ECB2-534B-AD4D-AA5F7D624C1A}"/>
   </bookViews>
@@ -1064,7 +1064,7 @@
   <dimension ref="B2:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1174,15 +1174,15 @@
         <v>-5.7264219999999998E-2</v>
       </c>
       <c r="G5" s="20">
-        <f>(MAX($F$4, F5) - MIN($F$4, F5))/MAX($F$4, F5)</f>
-        <v>-0.14371085470124276</v>
+        <f>(MAX(ABS($F$4), ABS(F5)) - MIN(ABS($F$4), ABS(F5)))/MAX(ABS($F$4), ABS(F5))</f>
+        <v>0.12565313524001007</v>
       </c>
       <c r="H5" s="15">
         <v>2</v>
       </c>
       <c r="I5" s="20">
-        <f>(MAX($F$3, F5) - MIN($F$3, F5))/MAX($F$3, F5)</f>
-        <v>-0.24722726918303706</v>
+        <f>(MAX(ABS($F$3), ABS(F5)) - MIN(ABS($F$3), ABS(F5)))/MAX(ABS($F$3), ABS(F5))</f>
+        <v>0.19822150725182322</v>
       </c>
       <c r="J5" s="15">
         <v>2</v>
@@ -1206,15 +1206,15 @@
         <v>-5.3999999999999999E-2</v>
       </c>
       <c r="G6" s="20">
-        <f>(MAX($F$4, F6) - MIN($F$4, F6))/MAX($F$4, F6)</f>
-        <v>-0.21284648148148144</v>
+        <f t="shared" ref="G6:G7" si="0">(MAX(ABS($F$4), ABS(F6)) - MIN(ABS($F$4), ABS(F6)))/MAX(ABS($F$4), ABS(F6))</f>
+        <v>0.17549334126895541</v>
       </c>
       <c r="H6" s="15">
         <v>3</v>
       </c>
       <c r="I6" s="20">
-        <f>(MAX($F$3, F6) - MIN($F$3, F6))/MAX($F$3, F6)</f>
-        <v>-0.17613184176583568</v>
+        <f t="shared" ref="I6:I7" si="1">(MAX(ABS($F$3), ABS(F6)) - MIN(ABS($F$3), ABS(F6)))/MAX(ABS($F$3), ABS(F6))</f>
+        <v>0.14975518518518521</v>
       </c>
       <c r="J6" s="15">
         <v>1</v>
@@ -1237,15 +1237,15 @@
         <v>-6.5493709999999997E-2</v>
       </c>
       <c r="G7" s="20">
-        <f>(MAX($F$4, F7) - MIN($F$4, F7))/MAX($F$4, F7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="15">
         <v>1</v>
       </c>
       <c r="I7" s="20">
-        <f>(MAX($F$3, F7) - MIN($F$3, F7))/MAX($F$3, F7)</f>
-        <v>-0.4264673660440283</v>
+        <f t="shared" si="1"/>
+        <v>0.29896748863364131</v>
       </c>
       <c r="J7" s="15">
         <v>3</v>
@@ -1291,15 +1291,15 @@
         <v>-7.9271709999999995E-2</v>
       </c>
       <c r="G9" s="20">
-        <f>(MAX($F$8, F9) - MIN($F$8, F9))/MAX($F$8, F9)</f>
-        <v>-1.5453799636969279</v>
+        <f>(MAX(ABS($F$8), ABS(F9)) - MIN(ABS($F$8), ABS(F9)))/MAX(ABS($F$8), ABS(F9))</f>
+        <v>0.60713134610064545</v>
       </c>
       <c r="H9" s="15">
         <v>4</v>
       </c>
       <c r="I9" s="20">
-        <f>(MAX($F$3, F9) - MIN($F$3, F9))/MAX($F$3, F9)</f>
-        <v>-0.72655522744865197</v>
+        <f>(MAX(ABS($F$3), ABS(F9)) - MIN(ABS($F$3), ABS(F9)))/MAX(ABS($F$3), ABS(F9))</f>
+        <v>0.42081204000771522</v>
       </c>
       <c r="J9" s="17">
         <v>3</v>
@@ -1322,15 +1322,15 @@
         <v>-2.5795769999999999E-2</v>
       </c>
       <c r="G10" s="20">
-        <f>(MAX($F$8, F10) - MIN($F$8, F10))/MAX($F$8, F10)</f>
-        <v>-0.20730530625757637</v>
+        <f t="shared" ref="G10:G12" si="2">(MAX(ABS($F$8), ABS(F10)) - MIN(ABS($F$8), ABS(F10)))/MAX(ABS($F$8), ABS(F10))</f>
+        <v>0.17170909891896738</v>
       </c>
       <c r="H10" s="15">
         <v>2</v>
       </c>
       <c r="I10" s="20">
-        <f>(MAX($F$3, F10) - MIN($F$3, F10))/MAX($F$3, F10)</f>
-        <v>-0.7798739870916821</v>
+        <f t="shared" ref="I10:I12" si="3">(MAX(ABS($F$3), ABS(F10)) - MIN(ABS($F$3), ABS(F10)))/MAX(ABS($F$3), ABS(F10))</f>
+        <v>0.43816247259503904</v>
       </c>
       <c r="J10" s="17">
         <v>4</v>
@@ -1353,15 +1353,15 @@
         <v>-3.7000249999999998E-2</v>
       </c>
       <c r="G11" s="20">
-        <f>(MAX($F$8, F11) - MIN($F$8, F11))/MAX($F$8, F11)</f>
-        <v>-0.18806185714648088</v>
+        <f t="shared" si="2"/>
+        <v>0.15829298450686141</v>
       </c>
       <c r="H11" s="15">
         <v>1</v>
       </c>
       <c r="I11" s="20">
-        <f>(MAX($F$3, F11) - MIN($F$3, F11))/MAX($F$3, F11)</f>
-        <v>-0.24088945344963883</v>
+        <f t="shared" si="3"/>
+        <v>0.19412644114266001</v>
       </c>
       <c r="J11" s="17">
         <v>1</v>
@@ -1384,15 +1384,15 @@
         <v>-6.3814620000000002E-2</v>
       </c>
       <c r="G12" s="20">
-        <f>(MAX($F$8, F12) - MIN($F$8, F12))/MAX($F$8, F12)</f>
-        <v>-1.0490595590650593</v>
+        <f t="shared" si="2"/>
+        <v>0.51197123793889232</v>
       </c>
       <c r="H12" s="15">
         <v>3</v>
       </c>
       <c r="I12" s="20">
-        <f>(MAX($F$3, F12) - MIN($F$3, F12))/MAX($F$3, F12)</f>
-        <v>-0.38989641763309141</v>
+        <f t="shared" si="3"/>
+        <v>0.28052192428631567</v>
       </c>
       <c r="J12" s="17">
         <v>2</v>

</xml_diff>